<commit_message>
Commiting current in case of need to revert
</commit_message>
<xml_diff>
--- a/sinnoh_cube.xlsx
+++ b/sinnoh_cube.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\levat\Documents\Tabletop Simulator\pokemon-legends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B39833-7622-4600-82F8-851CE3E45A03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9302CD9F-3AE6-40C1-9E18-C4400963BCFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12900" yWindow="4365" windowWidth="21600" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10350" yWindow="1020" windowWidth="21600" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sinnoh" sheetId="1" r:id="rId1"/>
@@ -3665,8 +3665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151:S151"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12979,17 +12979,16 @@
         <f t="shared" si="16"/>
         <v>8</v>
       </c>
-      <c r="Q147" s="1">
-        <f t="shared" si="16"/>
-        <v>12</v>
+      <c r="Q147" s="2">
+        <v>13</v>
       </c>
       <c r="R147" s="1">
         <f t="shared" si="14"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S147" s="1">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactored codebase to support a Language Module and a Config Module
</commit_message>
<xml_diff>
--- a/sinnoh_cube.xlsx
+++ b/sinnoh_cube.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lev\PycharmProjects\pokemon-legends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE5142F-F844-4030-9D25-D1F710F50D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF1E70B-3C2E-4978-8D4B-1DD00086B546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36255" yWindow="4245" windowWidth="21600" windowHeight="7200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41938,8 +41938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41F625C-F9FA-42D6-A0B3-21764E3166C5}">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42014,7 +42014,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="27">
-        <f>H2-G2</f>
+        <f t="shared" ref="I2:I65" si="0">H2-G2</f>
         <v>0</v>
       </c>
     </row>
@@ -42048,7 +42048,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="27">
-        <f>H3-G3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42082,7 +42082,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="26">
-        <f>H4-G4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42116,7 +42116,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="26">
-        <f>H5-G5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42149,7 +42149,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="26">
-        <f>H6-G6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42164,7 +42164,7 @@
         <v>20</v>
       </c>
       <c r="D7" s="29">
-        <f>IF(NOT(ISBLANK(C7)), IF(ISNUMBER(C7), ROUND((C7 - 5)/20, 0), C7), "")</f>
+        <f t="shared" ref="D7:D70" si="1">IF(NOT(ISBLANK(C7)), IF(ISNUMBER(C7), ROUND((C7 - 5)/20, 0), C7), "")</f>
         <v>1</v>
       </c>
       <c r="E7" s="26" t="s">
@@ -42183,7 +42183,7 @@
         <v>10</v>
       </c>
       <c r="I7" s="26">
-        <f>H7-G7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42198,7 +42198,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="29">
-        <f>IF(NOT(ISBLANK(C8)), IF(ISNUMBER(C8), ROUND((C8 - 5)/20, 0), C8), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E8" s="26" t="s">
@@ -42217,7 +42217,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="26">
-        <f>H8-G8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42232,7 +42232,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="25">
-        <f>IF(NOT(ISBLANK(C9)), IF(ISNUMBER(C9), ROUND((C9 - 5)/20, 0), C9), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E9" s="26" t="s">
@@ -42251,7 +42251,7 @@
         <v>11</v>
       </c>
       <c r="I9" s="27">
-        <f>H9-G9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42266,7 +42266,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="29">
-        <f>IF(NOT(ISBLANK(C10)), IF(ISNUMBER(C10), ROUND((C10 - 5)/20, 0), C10), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E10" s="26" t="s">
@@ -42285,7 +42285,7 @@
         <v>14</v>
       </c>
       <c r="I10" s="26">
-        <f>H10-G10</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -42300,7 +42300,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="29">
-        <f>IF(NOT(ISBLANK(C11)), IF(ISNUMBER(C11), ROUND((C11 - 5)/20, 0), C11), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E11" s="26" t="s">
@@ -42319,7 +42319,7 @@
         <v>10</v>
       </c>
       <c r="I11" s="26">
-        <f>H11-G11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42334,7 +42334,7 @@
         <v>20</v>
       </c>
       <c r="D12" s="29">
-        <f>IF(NOT(ISBLANK(C12)), IF(ISNUMBER(C12), ROUND((C12 - 5)/20, 0), C12), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E12" s="26" t="s">
@@ -42353,7 +42353,7 @@
         <v>14</v>
       </c>
       <c r="I12" s="26">
-        <f>H12-G12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42368,7 +42368,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="25">
-        <f>IF(NOT(ISBLANK(C13)), IF(ISNUMBER(C13), ROUND((C13 - 5)/20, 0), C13), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E13" s="26" t="s">
@@ -42387,7 +42387,7 @@
         <v>10</v>
       </c>
       <c r="I13" s="27">
-        <f>H13-G13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42402,7 +42402,7 @@
         <v>20</v>
       </c>
       <c r="D14" s="29">
-        <f>IF(NOT(ISBLANK(C14)), IF(ISNUMBER(C14), ROUND((C14 - 5)/20, 0), C14), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E14" s="26" t="s">
@@ -42421,7 +42421,7 @@
         <v>8</v>
       </c>
       <c r="I14" s="26">
-        <f>H14-G14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -42436,7 +42436,7 @@
         <v>20</v>
       </c>
       <c r="D15" s="29">
-        <f>IF(NOT(ISBLANK(C15)), IF(ISNUMBER(C15), ROUND((C15 - 5)/20, 0), C15), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E15" s="26" t="s">
@@ -42455,7 +42455,7 @@
         <v>12</v>
       </c>
       <c r="I15" s="26">
-        <f>H15-G15</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -42470,7 +42470,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="29">
-        <f>IF(NOT(ISBLANK(C16)), IF(ISNUMBER(C16), ROUND((C16 - 5)/20, 0), C16), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E16" s="26" t="s">
@@ -42489,7 +42489,7 @@
         <v>13</v>
       </c>
       <c r="I16" s="26">
-        <f>H16-G16</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -42504,7 +42504,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="29">
-        <f>IF(NOT(ISBLANK(C17)), IF(ISNUMBER(C17), ROUND((C17 - 5)/20, 0), C17), "")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E17" s="26" t="s">
@@ -42523,7 +42523,7 @@
         <v>10</v>
       </c>
       <c r="I17" s="27">
-        <f>H17-G17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42538,7 +42538,7 @@
         <v>40</v>
       </c>
       <c r="D18" s="25">
-        <f>IF(NOT(ISBLANK(C18)), IF(ISNUMBER(C18), ROUND((C18 - 5)/20, 0), C18), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E18" s="27" t="s">
@@ -42557,7 +42557,7 @@
         <v>12</v>
       </c>
       <c r="I18" s="27">
-        <f>H18-G18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42572,7 +42572,7 @@
         <v>40</v>
       </c>
       <c r="D19" s="29">
-        <f>IF(NOT(ISBLANK(C19)), IF(ISNUMBER(C19), ROUND((C19 - 5)/20, 0), C19), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E19" s="26" t="s">
@@ -42591,7 +42591,7 @@
         <v>18</v>
       </c>
       <c r="I19" s="26">
-        <f>H19-G19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42606,7 +42606,7 @@
         <v>40</v>
       </c>
       <c r="D20" s="29">
-        <f>IF(NOT(ISBLANK(C20)), IF(ISNUMBER(C20), ROUND((C20 - 5)/20, 0), C20), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E20" s="26" t="s">
@@ -42625,7 +42625,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="26">
-        <f>H20-G20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42640,7 +42640,7 @@
         <v>40</v>
       </c>
       <c r="D21" s="29">
-        <f>IF(NOT(ISBLANK(C21)), IF(ISNUMBER(C21), ROUND((C21 - 5)/20, 0), C21), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E21" s="26" t="s">
@@ -42659,7 +42659,7 @@
         <v>14</v>
       </c>
       <c r="I21" s="26">
-        <f>H21-G21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42674,7 +42674,7 @@
         <v>40</v>
       </c>
       <c r="D22" s="29">
-        <f>IF(NOT(ISBLANK(C22)), IF(ISNUMBER(C22), ROUND((C22 - 5)/20, 0), C22), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E22" s="26" t="s">
@@ -42693,7 +42693,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="26">
-        <f>H22-G22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42708,7 +42708,7 @@
         <v>40</v>
       </c>
       <c r="D23" s="25">
-        <f>IF(NOT(ISBLANK(C23)), IF(ISNUMBER(C23), ROUND((C23 - 5)/20, 0), C23), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E23" s="26" t="s">
@@ -42727,7 +42727,7 @@
         <v>15</v>
       </c>
       <c r="I23" s="27">
-        <f>H23-G23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42742,7 +42742,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="29">
-        <f>IF(NOT(ISBLANK(C24)), IF(ISNUMBER(C24), ROUND((C24 - 5)/20, 0), C24), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E24" s="26" t="s">
@@ -42761,7 +42761,7 @@
         <v>10</v>
       </c>
       <c r="I24" s="26">
-        <f>H24-G24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42776,7 +42776,7 @@
         <v>40</v>
       </c>
       <c r="D25" s="29">
-        <f>IF(NOT(ISBLANK(C25)), IF(ISNUMBER(C25), ROUND((C25 - 5)/20, 0), C25), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E25" s="26" t="s">
@@ -42795,7 +42795,7 @@
         <v>16</v>
       </c>
       <c r="I25" s="26">
-        <f>H25-G25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42810,7 +42810,7 @@
         <v>40</v>
       </c>
       <c r="D26" s="29">
-        <f>IF(NOT(ISBLANK(C26)), IF(ISNUMBER(C26), ROUND((C26 - 5)/20, 0), C26), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E26" s="27" t="s">
@@ -42829,7 +42829,7 @@
         <v>15</v>
       </c>
       <c r="I26" s="26">
-        <f>H26-G26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42844,7 +42844,7 @@
         <v>45</v>
       </c>
       <c r="D27" s="29">
-        <f>IF(NOT(ISBLANK(C27)), IF(ISNUMBER(C27), ROUND((C27 - 5)/20, 0), C27), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E27" s="26" t="s">
@@ -42863,7 +42863,7 @@
         <v>10</v>
       </c>
       <c r="I27" s="26">
-        <f>H27-G27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42878,7 +42878,7 @@
         <v>40</v>
       </c>
       <c r="D28" s="29">
-        <f>IF(NOT(ISBLANK(C28)), IF(ISNUMBER(C28), ROUND((C28 - 5)/20, 0), C28), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E28" s="26" t="s">
@@ -42897,7 +42897,7 @@
         <v>8</v>
       </c>
       <c r="I28" s="26">
-        <f>H28-G28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42912,7 +42912,7 @@
         <v>40</v>
       </c>
       <c r="D29" s="29">
-        <f>IF(NOT(ISBLANK(C29)), IF(ISNUMBER(C29), ROUND((C29 - 5)/20, 0), C29), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E29" s="26" t="s">
@@ -42931,7 +42931,7 @@
         <v>13</v>
       </c>
       <c r="I29" s="26">
-        <f>H29-G29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42946,7 +42946,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="29">
-        <f>IF(NOT(ISBLANK(C30)), IF(ISNUMBER(C30), ROUND((C30 - 5)/20, 0), C30), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E30" s="26" t="s">
@@ -42965,7 +42965,7 @@
         <v>16</v>
       </c>
       <c r="I30" s="26">
-        <f>H30-G30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -42980,7 +42980,7 @@
         <v>40</v>
       </c>
       <c r="D31" s="25">
-        <f>IF(NOT(ISBLANK(C31)), IF(ISNUMBER(C31), ROUND((C31 - 5)/20, 0), C31), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E31" s="26" t="s">
@@ -42999,7 +42999,7 @@
         <v>14</v>
       </c>
       <c r="I31" s="27">
-        <f>H31-G31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43014,7 +43014,7 @@
         <v>40</v>
       </c>
       <c r="D32" s="25">
-        <f>IF(NOT(ISBLANK(C32)), IF(ISNUMBER(C32), ROUND((C32 - 5)/20, 0), C32), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E32" s="26" t="s">
@@ -43033,7 +43033,7 @@
         <v>17</v>
       </c>
       <c r="I32" s="27">
-        <f>H32-G32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43048,7 +43048,7 @@
         <v>40</v>
       </c>
       <c r="D33" s="25">
-        <f>IF(NOT(ISBLANK(C33)), IF(ISNUMBER(C33), ROUND((C33 - 5)/20, 0), C33), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E33" s="26" t="s">
@@ -43067,7 +43067,7 @@
         <v>11</v>
       </c>
       <c r="I33" s="27">
-        <f>H33-G33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -43082,7 +43082,7 @@
         <v>50</v>
       </c>
       <c r="D34" s="29">
-        <f>IF(NOT(ISBLANK(C34)), IF(ISNUMBER(C34), ROUND((C34 - 5)/20, 0), C34), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E34" s="26" t="s">
@@ -43101,7 +43101,7 @@
         <v>11</v>
       </c>
       <c r="I34" s="26">
-        <f>H34-G34</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -43116,7 +43116,7 @@
         <v>40</v>
       </c>
       <c r="D35" s="29">
-        <f>IF(NOT(ISBLANK(C35)), IF(ISNUMBER(C35), ROUND((C35 - 5)/20, 0), C35), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E35" s="26" t="s">
@@ -43135,7 +43135,7 @@
         <v>10</v>
       </c>
       <c r="I35" s="26">
-        <f>H35-G35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43150,7 +43150,7 @@
         <v>40</v>
       </c>
       <c r="D36" s="29">
-        <f>IF(NOT(ISBLANK(C36)), IF(ISNUMBER(C36), ROUND((C36 - 5)/20, 0), C36), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E36" s="26" t="s">
@@ -43169,7 +43169,7 @@
         <v>21</v>
       </c>
       <c r="I36" s="26">
-        <f>H36-G36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43184,7 +43184,7 @@
         <v>40</v>
       </c>
       <c r="D37" s="29">
-        <f>IF(NOT(ISBLANK(C37)), IF(ISNUMBER(C37), ROUND((C37 - 5)/20, 0), C37), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E37" s="26" t="s">
@@ -43203,7 +43203,7 @@
         <v>11</v>
       </c>
       <c r="I37" s="26">
-        <f>H37-G37</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -43218,7 +43218,7 @@
         <v>40</v>
       </c>
       <c r="D38" s="29">
-        <f>IF(NOT(ISBLANK(C38)), IF(ISNUMBER(C38), ROUND((C38 - 5)/20, 0), C38), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E38" s="26" t="s">
@@ -43237,7 +43237,7 @@
         <v>13</v>
       </c>
       <c r="I38" s="26">
-        <f>H38-G38</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -43252,7 +43252,7 @@
         <v>50</v>
       </c>
       <c r="D39" s="29">
-        <f>IF(NOT(ISBLANK(C39)), IF(ISNUMBER(C39), ROUND((C39 - 5)/20, 0), C39), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E39" s="26" t="s">
@@ -43271,7 +43271,7 @@
         <v>9</v>
       </c>
       <c r="I39" s="26">
-        <f>H39-G39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43286,7 +43286,7 @@
         <v>40</v>
       </c>
       <c r="D40" s="25">
-        <f>IF(NOT(ISBLANK(C40)), IF(ISNUMBER(C40), ROUND((C40 - 5)/20, 0), C40), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E40" s="27" t="s">
@@ -43305,7 +43305,7 @@
         <v>9</v>
       </c>
       <c r="I40" s="27">
-        <f>H40-G40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43320,7 +43320,7 @@
         <v>35</v>
       </c>
       <c r="D41" s="29">
-        <f>IF(NOT(ISBLANK(C41)), IF(ISNUMBER(C41), ROUND((C41 - 5)/20, 0), C41), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E41" s="26" t="s">
@@ -43339,7 +43339,7 @@
         <v>13</v>
       </c>
       <c r="I41" s="26">
-        <f>H41-G41</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43354,7 +43354,7 @@
         <v>35</v>
       </c>
       <c r="D42" s="29">
-        <f>IF(NOT(ISBLANK(C42)), IF(ISNUMBER(C42), ROUND((C42 - 5)/20, 0), C42), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E42" s="26" t="s">
@@ -43373,7 +43373,7 @@
         <v>11</v>
       </c>
       <c r="I42" s="26">
-        <f>H42-G42</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -43388,7 +43388,7 @@
         <v>40</v>
       </c>
       <c r="D43" s="25">
-        <f>IF(NOT(ISBLANK(C43)), IF(ISNUMBER(C43), ROUND((C43 - 5)/20, 0), C43), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E43" s="26" t="s">
@@ -43407,7 +43407,7 @@
         <v>12</v>
       </c>
       <c r="I43" s="27">
-        <f>H43-G43</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43422,7 +43422,7 @@
         <v>40</v>
       </c>
       <c r="D44" s="25">
-        <f>IF(NOT(ISBLANK(C44)), IF(ISNUMBER(C44), ROUND((C44 - 5)/20, 0), C44), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E44" s="26" t="s">
@@ -43441,7 +43441,7 @@
         <v>14</v>
       </c>
       <c r="I44" s="27">
-        <f>H44-G44</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43456,7 +43456,7 @@
         <v>50</v>
       </c>
       <c r="D45" s="25">
-        <f>IF(NOT(ISBLANK(C45)), IF(ISNUMBER(C45), ROUND((C45 - 5)/20, 0), C45), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E45" s="26" t="s">
@@ -43475,7 +43475,7 @@
         <v>10</v>
       </c>
       <c r="I45" s="27">
-        <f>H45-G45</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43490,7 +43490,7 @@
         <v>35</v>
       </c>
       <c r="D46" s="29">
-        <f>IF(NOT(ISBLANK(C46)), IF(ISNUMBER(C46), ROUND((C46 - 5)/20, 0), C46), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E46" s="26" t="s">
@@ -43509,7 +43509,7 @@
         <v>10</v>
       </c>
       <c r="I46" s="26">
-        <f>H46-G46</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43524,7 +43524,7 @@
         <v>50</v>
       </c>
       <c r="D47" s="29">
-        <f>IF(NOT(ISBLANK(C47)), IF(ISNUMBER(C47), ROUND((C47 - 5)/20, 0), C47), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E47" s="26" t="s">
@@ -43543,7 +43543,7 @@
         <v>13</v>
       </c>
       <c r="I47" s="26">
-        <f>H47-G47</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -43558,7 +43558,7 @@
         <v>40</v>
       </c>
       <c r="D48" s="29">
-        <f>IF(NOT(ISBLANK(C48)), IF(ISNUMBER(C48), ROUND((C48 - 5)/20, 0), C48), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E48" s="26" t="s">
@@ -43577,7 +43577,7 @@
         <v>11</v>
       </c>
       <c r="I48" s="26">
-        <f>H48-G48</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -43592,7 +43592,7 @@
         <v>40</v>
       </c>
       <c r="D49" s="29">
-        <f>IF(NOT(ISBLANK(C49)), IF(ISNUMBER(C49), ROUND((C49 - 5)/20, 0), C49), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E49" s="26" t="s">
@@ -43611,7 +43611,7 @@
         <v>9</v>
       </c>
       <c r="I49" s="26">
-        <f>H49-G49</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -43626,7 +43626,7 @@
         <v>40</v>
       </c>
       <c r="D50" s="25">
-        <f>IF(NOT(ISBLANK(C50)), IF(ISNUMBER(C50), ROUND((C50 - 5)/20, 0), C50), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E50" s="26" t="s">
@@ -43645,7 +43645,7 @@
         <v>10</v>
       </c>
       <c r="I50" s="27">
-        <f>H50-G50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43660,7 +43660,7 @@
         <v>50</v>
       </c>
       <c r="D51" s="25">
-        <f>IF(NOT(ISBLANK(C51)), IF(ISNUMBER(C51), ROUND((C51 - 5)/20, 0), C51), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E51" s="26" t="s">
@@ -43679,7 +43679,7 @@
         <v>7</v>
       </c>
       <c r="I51" s="27">
-        <f>H51-G51</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43694,7 +43694,7 @@
         <v>40</v>
       </c>
       <c r="D52" s="29">
-        <f>IF(NOT(ISBLANK(C52)), IF(ISNUMBER(C52), ROUND((C52 - 5)/20, 0), C52), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E52" s="26" t="s">
@@ -43713,7 +43713,7 @@
         <v>16</v>
       </c>
       <c r="I52" s="26">
-        <f>H52-G52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43728,7 +43728,7 @@
         <v>40</v>
       </c>
       <c r="D53" s="25">
-        <f>IF(NOT(ISBLANK(C53)), IF(ISNUMBER(C53), ROUND((C53 - 5)/20, 0), C53), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E53" s="26" t="s">
@@ -43747,7 +43747,7 @@
         <v>10</v>
       </c>
       <c r="I53" s="27">
-        <f>H53-G53</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43762,7 +43762,7 @@
         <v>40</v>
       </c>
       <c r="D54" s="29">
-        <f>IF(NOT(ISBLANK(C54)), IF(ISNUMBER(C54), ROUND((C54 - 5)/20, 0), C54), "")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E54" s="26" t="s">
@@ -43781,7 +43781,7 @@
         <v>13</v>
       </c>
       <c r="I54" s="26">
-        <f>H54-G54</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43796,7 +43796,7 @@
         <v>60</v>
       </c>
       <c r="D55" s="29">
-        <f>IF(NOT(ISBLANK(C55)), IF(ISNUMBER(C55), ROUND((C55 - 5)/20, 0), C55), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E55" s="26" t="s">
@@ -43815,7 +43815,7 @@
         <v>15</v>
       </c>
       <c r="I55" s="26">
-        <f>H55-G55</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -43830,7 +43830,7 @@
         <v>60</v>
       </c>
       <c r="D56" s="29">
-        <f>IF(NOT(ISBLANK(C56)), IF(ISNUMBER(C56), ROUND((C56 - 5)/20, 0), C56), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E56" s="26" t="s">
@@ -43849,7 +43849,7 @@
         <v>12</v>
       </c>
       <c r="I56" s="26">
-        <f>H56-G56</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43864,7 +43864,7 @@
         <v>55</v>
       </c>
       <c r="D57" s="29">
-        <f>IF(NOT(ISBLANK(C57)), IF(ISNUMBER(C57), ROUND((C57 - 5)/20, 0), C57), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E57" s="26" t="s">
@@ -43883,7 +43883,7 @@
         <v>11</v>
       </c>
       <c r="I57" s="26">
-        <f>H57-G57</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43898,7 +43898,7 @@
         <v>60</v>
       </c>
       <c r="D58" s="29">
-        <f>IF(NOT(ISBLANK(C58)), IF(ISNUMBER(C58), ROUND((C58 - 5)/20, 0), C58), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E58" s="27" t="s">
@@ -43917,7 +43917,7 @@
         <v>11</v>
       </c>
       <c r="I58" s="26">
-        <f>H58-G58</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -43932,7 +43932,7 @@
         <v>60</v>
       </c>
       <c r="D59" s="29">
-        <f>IF(NOT(ISBLANK(C59)), IF(ISNUMBER(C59), ROUND((C59 - 5)/20, 0), C59), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E59" s="26" t="s">
@@ -43951,7 +43951,7 @@
         <v>16</v>
       </c>
       <c r="I59" s="26">
-        <f>H59-G59</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -43966,7 +43966,7 @@
         <v>55</v>
       </c>
       <c r="D60" s="29">
-        <f>IF(NOT(ISBLANK(C60)), IF(ISNUMBER(C60), ROUND((C60 - 5)/20, 0), C60), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E60" s="26" t="s">
@@ -43985,7 +43985,7 @@
         <v>10</v>
       </c>
       <c r="I60" s="26">
-        <f>H60-G60</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -44000,7 +44000,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="29">
-        <f>IF(NOT(ISBLANK(C61)), IF(ISNUMBER(C61), ROUND((C61 - 5)/20, 0), C61), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E61" s="26" t="s">
@@ -44019,7 +44019,7 @@
         <v>16</v>
       </c>
       <c r="I61" s="26">
-        <f>H61-G61</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -44034,7 +44034,7 @@
         <v>65</v>
       </c>
       <c r="D62" s="29">
-        <f>IF(NOT(ISBLANK(C62)), IF(ISNUMBER(C62), ROUND((C62 - 5)/20, 0), C62), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E62" s="26" t="s">
@@ -44053,7 +44053,7 @@
         <v>12</v>
       </c>
       <c r="I62" s="26">
-        <f>H62-G62</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -44068,7 +44068,7 @@
         <v>60</v>
       </c>
       <c r="D63" s="29">
-        <f>IF(NOT(ISBLANK(C63)), IF(ISNUMBER(C63), ROUND((C63 - 5)/20, 0), C63), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E63" s="26" t="s">
@@ -44087,7 +44087,7 @@
         <v>14</v>
       </c>
       <c r="I63" s="26">
-        <f>H63-G63</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -44102,7 +44102,7 @@
         <v>60</v>
       </c>
       <c r="D64" s="29">
-        <f>IF(NOT(ISBLANK(C64)), IF(ISNUMBER(C64), ROUND((C64 - 5)/20, 0), C64), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E64" s="26" t="s">
@@ -44121,7 +44121,7 @@
         <v>14</v>
       </c>
       <c r="I64" s="26">
-        <f>H64-G64</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -44136,7 +44136,7 @@
         <v>65</v>
       </c>
       <c r="D65" s="29">
-        <f>IF(NOT(ISBLANK(C65)), IF(ISNUMBER(C65), ROUND((C65 - 5)/20, 0), C65), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E65" s="26" t="s">
@@ -44155,7 +44155,7 @@
         <v>15</v>
       </c>
       <c r="I65" s="26">
-        <f>H65-G65</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -44170,7 +44170,7 @@
         <v>60</v>
       </c>
       <c r="D66" s="29">
-        <f>IF(NOT(ISBLANK(C66)), IF(ISNUMBER(C66), ROUND((C66 - 5)/20, 0), C66), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E66" s="26" t="s">
@@ -44189,7 +44189,7 @@
         <v>17</v>
       </c>
       <c r="I66" s="26">
-        <f>H66-G66</f>
+        <f t="shared" ref="I66:I129" si="2">H66-G66</f>
         <v>0</v>
       </c>
     </row>
@@ -44204,7 +44204,7 @@
         <v>70</v>
       </c>
       <c r="D67" s="29">
-        <f>IF(NOT(ISBLANK(C67)), IF(ISNUMBER(C67), ROUND((C67 - 5)/20, 0), C67), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E67" s="26" t="s">
@@ -44223,7 +44223,7 @@
         <v>14</v>
       </c>
       <c r="I67" s="26">
-        <f>H67-G67</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -44238,7 +44238,7 @@
         <v>65</v>
       </c>
       <c r="D68" s="29">
-        <f>IF(NOT(ISBLANK(C68)), IF(ISNUMBER(C68), ROUND((C68 - 5)/20, 0), C68), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E68" s="26" t="s">
@@ -44257,7 +44257,7 @@
         <v>15</v>
       </c>
       <c r="I68" s="26">
-        <f>H68-G68</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -44272,7 +44272,7 @@
         <v>65</v>
       </c>
       <c r="D69" s="29">
-        <f>IF(NOT(ISBLANK(C69)), IF(ISNUMBER(C69), ROUND((C69 - 5)/20, 0), C69), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E69" s="26" t="s">
@@ -44291,7 +44291,7 @@
         <v>14</v>
       </c>
       <c r="I69" s="26">
-        <f>H69-G69</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44306,7 +44306,7 @@
         <v>55</v>
       </c>
       <c r="D70" s="29">
-        <f>IF(NOT(ISBLANK(C70)), IF(ISNUMBER(C70), ROUND((C70 - 5)/20, 0), C70), "")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E70" s="26" t="s">
@@ -44325,7 +44325,7 @@
         <v>16</v>
       </c>
       <c r="I70" s="26">
-        <f>H70-G70</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44340,7 +44340,7 @@
         <v>60</v>
       </c>
       <c r="D71" s="25">
-        <f>IF(NOT(ISBLANK(C71)), IF(ISNUMBER(C71), ROUND((C71 - 5)/20, 0), C71), "")</f>
+        <f t="shared" ref="D71:D134" si="3">IF(NOT(ISBLANK(C71)), IF(ISNUMBER(C71), ROUND((C71 - 5)/20, 0), C71), "")</f>
         <v>3</v>
       </c>
       <c r="E71" s="26" t="s">
@@ -44359,7 +44359,7 @@
         <v>15</v>
       </c>
       <c r="I71" s="27">
-        <f>H71-G71</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44374,7 +44374,7 @@
         <v>60</v>
       </c>
       <c r="D72" s="29">
-        <f>IF(NOT(ISBLANK(C72)), IF(ISNUMBER(C72), ROUND((C72 - 5)/20, 0), C72), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E72" s="26" t="s">
@@ -44393,7 +44393,7 @@
         <v>28</v>
       </c>
       <c r="I72" s="26">
-        <f>H72-G72</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44408,7 +44408,7 @@
         <v>60</v>
       </c>
       <c r="D73" s="29">
-        <f>IF(NOT(ISBLANK(C73)), IF(ISNUMBER(C73), ROUND((C73 - 5)/20, 0), C73), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E73" s="26" t="s">
@@ -44427,7 +44427,7 @@
         <v>28</v>
       </c>
       <c r="I73" s="26">
-        <f>H73-G73</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44442,7 +44442,7 @@
         <v>70</v>
       </c>
       <c r="D74" s="29">
-        <f>IF(NOT(ISBLANK(C74)), IF(ISNUMBER(C74), ROUND((C74 - 5)/20, 0), C74), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E74" s="26" t="s">
@@ -44461,7 +44461,7 @@
         <v>17</v>
       </c>
       <c r="I74" s="26">
-        <f>H74-G74</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44476,7 +44476,7 @@
         <v>60</v>
       </c>
       <c r="D75" s="29">
-        <f>IF(NOT(ISBLANK(C75)), IF(ISNUMBER(C75), ROUND((C75 - 5)/20, 0), C75), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E75" s="26" t="s">
@@ -44495,7 +44495,7 @@
         <v>28</v>
       </c>
       <c r="I75" s="26">
-        <f>H75-G75</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44510,7 +44510,7 @@
         <v>65</v>
       </c>
       <c r="D76" s="29">
-        <f>IF(NOT(ISBLANK(C76)), IF(ISNUMBER(C76), ROUND((C76 - 5)/20, 0), C76), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E76" s="26" t="s">
@@ -44529,7 +44529,7 @@
         <v>15</v>
       </c>
       <c r="I76" s="26">
-        <f>H76-G76</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44544,7 +44544,7 @@
         <v>60</v>
       </c>
       <c r="D77" s="29">
-        <f>IF(NOT(ISBLANK(C77)), IF(ISNUMBER(C77), ROUND((C77 - 5)/20, 0), C77), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E77" s="26" t="s">
@@ -44563,7 +44563,7 @@
         <v>16</v>
       </c>
       <c r="I77" s="26">
-        <f>H77-G77</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44578,7 +44578,7 @@
         <v>60</v>
       </c>
       <c r="D78" s="29">
-        <f>IF(NOT(ISBLANK(C78)), IF(ISNUMBER(C78), ROUND((C78 - 5)/20, 0), C78), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E78" s="26" t="s">
@@ -44597,7 +44597,7 @@
         <v>16</v>
       </c>
       <c r="I78" s="26">
-        <f>H78-G78</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44612,7 +44612,7 @@
         <v>55</v>
       </c>
       <c r="D79" s="29">
-        <f>IF(NOT(ISBLANK(C79)), IF(ISNUMBER(C79), ROUND((C79 - 5)/20, 0), C79), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E79" s="26" t="s">
@@ -44631,7 +44631,7 @@
         <v>14</v>
       </c>
       <c r="I79" s="26">
-        <f>H79-G79</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -44646,7 +44646,7 @@
         <v>60</v>
       </c>
       <c r="D80" s="29">
-        <f>IF(NOT(ISBLANK(C80)), IF(ISNUMBER(C80), ROUND((C80 - 5)/20, 0), C80), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E80" s="26" t="s">
@@ -44665,7 +44665,7 @@
         <v>15</v>
       </c>
       <c r="I80" s="26">
-        <f>H80-G80</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -44680,7 +44680,7 @@
         <v>70</v>
       </c>
       <c r="D81" s="29">
-        <f>IF(NOT(ISBLANK(C81)), IF(ISNUMBER(C81), ROUND((C81 - 5)/20, 0), C81), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E81" s="26" t="s">
@@ -44699,7 +44699,7 @@
         <v>11</v>
       </c>
       <c r="I81" s="26">
-        <f>H81-G81</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44714,7 +44714,7 @@
         <v>70</v>
       </c>
       <c r="D82" s="29">
-        <f>IF(NOT(ISBLANK(C82)), IF(ISNUMBER(C82), ROUND((C82 - 5)/20, 0), C82), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E82" s="26" t="s">
@@ -44733,7 +44733,7 @@
         <v>10</v>
       </c>
       <c r="I82" s="26">
-        <f>H82-G82</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44748,7 +44748,7 @@
         <v>60</v>
       </c>
       <c r="D83" s="29">
-        <f>IF(NOT(ISBLANK(C83)), IF(ISNUMBER(C83), ROUND((C83 - 5)/20, 0), C83), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E83" s="26" t="s">
@@ -44767,7 +44767,7 @@
         <v>17</v>
       </c>
       <c r="I83" s="26">
-        <f>H83-G83</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44782,7 +44782,7 @@
         <v>60</v>
       </c>
       <c r="D84" s="29">
-        <f>IF(NOT(ISBLANK(C84)), IF(ISNUMBER(C84), ROUND((C84 - 5)/20, 0), C84), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E84" s="26" t="s">
@@ -44801,7 +44801,7 @@
         <v>28</v>
       </c>
       <c r="I84" s="26">
-        <f>H84-G84</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44816,7 +44816,7 @@
         <v>60</v>
       </c>
       <c r="D85" s="29">
-        <f>IF(NOT(ISBLANK(C85)), IF(ISNUMBER(C85), ROUND((C85 - 5)/20, 0), C85), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E85" s="26" t="s">
@@ -44835,7 +44835,7 @@
         <v>14</v>
       </c>
       <c r="I85" s="26">
-        <f>H85-G85</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -44850,7 +44850,7 @@
         <v>65</v>
       </c>
       <c r="D86" s="29">
-        <f>IF(NOT(ISBLANK(C86)), IF(ISNUMBER(C86), ROUND((C86 - 5)/20, 0), C86), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E86" s="26" t="s">
@@ -44869,7 +44869,7 @@
         <v>11</v>
       </c>
       <c r="I86" s="26">
-        <f>H86-G86</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -44884,7 +44884,7 @@
         <v>70</v>
       </c>
       <c r="D87" s="29">
-        <f>IF(NOT(ISBLANK(C87)), IF(ISNUMBER(C87), ROUND((C87 - 5)/20, 0), C87), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E87" s="26" t="s">
@@ -44903,7 +44903,7 @@
         <v>11</v>
       </c>
       <c r="I87" s="26">
-        <f>H87-G87</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -44918,7 +44918,7 @@
         <v>60</v>
       </c>
       <c r="D88" s="29">
-        <f>IF(NOT(ISBLANK(C88)), IF(ISNUMBER(C88), ROUND((C88 - 5)/20, 0), C88), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E88" s="26" t="s">
@@ -44937,7 +44937,7 @@
         <v>14</v>
       </c>
       <c r="I88" s="26">
-        <f>H88-G88</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -44952,7 +44952,7 @@
         <v>65</v>
       </c>
       <c r="D89" s="29">
-        <f>IF(NOT(ISBLANK(C89)), IF(ISNUMBER(C89), ROUND((C89 - 5)/20, 0), C89), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E89" s="26" t="s">
@@ -44971,7 +44971,7 @@
         <v>11</v>
       </c>
       <c r="I89" s="26">
-        <f>H89-G89</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -44986,7 +44986,7 @@
         <v>60</v>
       </c>
       <c r="D90" s="25">
-        <f>IF(NOT(ISBLANK(C90)), IF(ISNUMBER(C90), ROUND((C90 - 5)/20, 0), C90), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E90" s="26" t="s">
@@ -45005,7 +45005,7 @@
         <v>13</v>
       </c>
       <c r="I90" s="27">
-        <f>H90-G90</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -45020,7 +45020,7 @@
         <v>60</v>
       </c>
       <c r="D91" s="25">
-        <f>IF(NOT(ISBLANK(C91)), IF(ISNUMBER(C91), ROUND((C91 - 5)/20, 0), C91), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E91" s="27" t="s">
@@ -45039,7 +45039,7 @@
         <v>16</v>
       </c>
       <c r="I91" s="27">
-        <f>H91-G91</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45054,7 +45054,7 @@
         <v>70</v>
       </c>
       <c r="D92" s="25">
-        <f>IF(NOT(ISBLANK(C92)), IF(ISNUMBER(C92), ROUND((C92 - 5)/20, 0), C92), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E92" s="26" t="s">
@@ -45073,7 +45073,7 @@
         <v>13</v>
       </c>
       <c r="I92" s="27">
-        <f>H92-G92</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45088,7 +45088,7 @@
         <v>60</v>
       </c>
       <c r="D93" s="29">
-        <f>IF(NOT(ISBLANK(C93)), IF(ISNUMBER(C93), ROUND((C93 - 5)/20, 0), C93), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E93" s="26" t="s">
@@ -45107,7 +45107,7 @@
         <v>17</v>
       </c>
       <c r="I93" s="26">
-        <f>H93-G93</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45122,7 +45122,7 @@
         <v>60</v>
       </c>
       <c r="D94" s="29">
-        <f>IF(NOT(ISBLANK(C94)), IF(ISNUMBER(C94), ROUND((C94 - 5)/20, 0), C94), "")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="E94" s="26" t="s">
@@ -45141,7 +45141,7 @@
         <v>14</v>
       </c>
       <c r="I94" s="26">
-        <f>H94-G94</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45156,7 +45156,7 @@
         <v>75</v>
       </c>
       <c r="D95" s="29">
-        <f>IF(NOT(ISBLANK(C95)), IF(ISNUMBER(C95), ROUND((C95 - 5)/20, 0), C95), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E95" s="26" t="s">
@@ -45175,7 +45175,7 @@
         <v>16</v>
       </c>
       <c r="I95" s="26">
-        <f>H95-G95</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45190,7 +45190,7 @@
         <v>90</v>
       </c>
       <c r="D96" s="25">
-        <f>IF(NOT(ISBLANK(C96)), IF(ISNUMBER(C96), ROUND((C96 - 5)/20, 0), C96), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E96" s="26" t="s">
@@ -45209,7 +45209,7 @@
         <v>20</v>
       </c>
       <c r="I96" s="27">
-        <f>H96-G96</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45224,7 +45224,7 @@
         <v>75</v>
       </c>
       <c r="D97" s="29">
-        <f>IF(NOT(ISBLANK(C97)), IF(ISNUMBER(C97), ROUND((C97 - 5)/20, 0), C97), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E97" s="26" t="s">
@@ -45243,7 +45243,7 @@
         <v>28</v>
       </c>
       <c r="I97" s="26">
-        <f>H97-G97</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45258,7 +45258,7 @@
         <v>90</v>
       </c>
       <c r="D98" s="29">
-        <f>IF(NOT(ISBLANK(C98)), IF(ISNUMBER(C98), ROUND((C98 - 5)/20, 0), C98), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E98" s="26" t="s">
@@ -45277,7 +45277,7 @@
         <v>15</v>
       </c>
       <c r="I98" s="26">
-        <f>H98-G98</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45292,7 +45292,7 @@
         <v>75</v>
       </c>
       <c r="D99" s="29">
-        <f>IF(NOT(ISBLANK(C99)), IF(ISNUMBER(C99), ROUND((C99 - 5)/20, 0), C99), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E99" s="26" t="s">
@@ -45311,7 +45311,7 @@
         <v>20</v>
       </c>
       <c r="I99" s="26">
-        <f>H99-G99</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -45326,7 +45326,7 @@
         <v>75</v>
       </c>
       <c r="D100" s="29">
-        <f>IF(NOT(ISBLANK(C100)), IF(ISNUMBER(C100), ROUND((C100 - 5)/20, 0), C100), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E100" s="26" t="s">
@@ -45345,7 +45345,7 @@
         <v>19</v>
       </c>
       <c r="I100" s="26">
-        <f>H100-G100</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -45360,7 +45360,7 @@
         <v>85</v>
       </c>
       <c r="D101" s="29">
-        <f>IF(NOT(ISBLANK(C101)), IF(ISNUMBER(C101), ROUND((C101 - 5)/20, 0), C101), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E101" s="26" t="s">
@@ -45379,7 +45379,7 @@
         <v>18</v>
       </c>
       <c r="I101" s="26">
-        <f>H101-G101</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -45394,7 +45394,7 @@
         <v>75</v>
       </c>
       <c r="D102" s="29">
-        <f>IF(NOT(ISBLANK(C102)), IF(ISNUMBER(C102), ROUND((C102 - 5)/20, 0), C102), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E102" s="26" t="s">
@@ -45413,7 +45413,7 @@
         <v>17</v>
       </c>
       <c r="I102" s="26">
-        <f>H102-G102</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -45428,7 +45428,7 @@
         <v>75</v>
       </c>
       <c r="D103" s="25">
-        <f>IF(NOT(ISBLANK(C103)), IF(ISNUMBER(C103), ROUND((C103 - 5)/20, 0), C103), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E103" s="26" t="s">
@@ -45447,7 +45447,7 @@
         <v>16</v>
       </c>
       <c r="I103" s="27">
-        <f>H103-G103</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45462,7 +45462,7 @@
         <v>75</v>
       </c>
       <c r="D104" s="29">
-        <f>IF(NOT(ISBLANK(C104)), IF(ISNUMBER(C104), ROUND((C104 - 5)/20, 0), C104), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E104" s="26" t="s">
@@ -45481,7 +45481,7 @@
         <v>16</v>
       </c>
       <c r="I104" s="26">
-        <f>H104-G104</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45496,7 +45496,7 @@
         <v>80</v>
       </c>
       <c r="D105" s="29">
-        <f>IF(NOT(ISBLANK(C105)), IF(ISNUMBER(C105), ROUND((C105 - 5)/20, 0), C105), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E105" s="26" t="s">
@@ -45515,7 +45515,7 @@
         <v>18</v>
       </c>
       <c r="I105" s="26">
-        <f>H105-G105</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -45530,7 +45530,7 @@
         <v>75</v>
       </c>
       <c r="D106" s="29">
-        <f>IF(NOT(ISBLANK(C106)), IF(ISNUMBER(C106), ROUND((C106 - 5)/20, 0), C106), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E106" s="26" t="s">
@@ -45549,7 +45549,7 @@
         <v>16</v>
       </c>
       <c r="I106" s="26">
-        <f>H106-G106</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45564,7 +45564,7 @@
         <v>80</v>
       </c>
       <c r="D107" s="29">
-        <f>IF(NOT(ISBLANK(C107)), IF(ISNUMBER(C107), ROUND((C107 - 5)/20, 0), C107), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E107" s="26" t="s">
@@ -45583,7 +45583,7 @@
         <v>18</v>
       </c>
       <c r="I107" s="26">
-        <f>H107-G107</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45598,7 +45598,7 @@
         <v>80</v>
       </c>
       <c r="D108" s="25">
-        <f>IF(NOT(ISBLANK(C108)), IF(ISNUMBER(C108), ROUND((C108 - 5)/20, 0), C108), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E108" s="27" t="s">
@@ -45617,7 +45617,7 @@
         <v>15</v>
       </c>
       <c r="I108" s="27">
-        <f>H108-G108</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45632,7 +45632,7 @@
         <v>80</v>
       </c>
       <c r="D109" s="29">
-        <f>IF(NOT(ISBLANK(C109)), IF(ISNUMBER(C109), ROUND((C109 - 5)/20, 0), C109), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E109" s="26" t="s">
@@ -45651,7 +45651,7 @@
         <v>18</v>
       </c>
       <c r="I109" s="26">
-        <f>H109-G109</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45666,7 +45666,7 @@
         <v>80</v>
       </c>
       <c r="D110" s="25">
-        <f>IF(NOT(ISBLANK(C110)), IF(ISNUMBER(C110), ROUND((C110 - 5)/20, 0), C110), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E110" s="26" t="s">
@@ -45685,7 +45685,7 @@
         <v>16</v>
       </c>
       <c r="I110" s="27">
-        <f>H110-G110</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45700,7 +45700,7 @@
         <v>80</v>
       </c>
       <c r="D111" s="25">
-        <f>IF(NOT(ISBLANK(C111)), IF(ISNUMBER(C111), ROUND((C111 - 5)/20, 0), C111), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E111" s="26" t="s">
@@ -45719,7 +45719,7 @@
         <v>0</v>
       </c>
       <c r="I111" s="27">
-        <f>H111-G111</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45734,7 +45734,7 @@
         <v>80</v>
       </c>
       <c r="D112" s="25">
-        <f>IF(NOT(ISBLANK(C112)), IF(ISNUMBER(C112), ROUND((C112 - 5)/20, 0), C112), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E112" s="26" t="s">
@@ -45753,7 +45753,7 @@
         <v>0</v>
       </c>
       <c r="I112" s="27">
-        <f>H112-G112</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45768,7 +45768,7 @@
         <v>80</v>
       </c>
       <c r="D113" s="25">
-        <f>IF(NOT(ISBLANK(C113)), IF(ISNUMBER(C113), ROUND((C113 - 5)/20, 0), C113), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E113" s="26" t="s">
@@ -45787,7 +45787,7 @@
         <v>0</v>
       </c>
       <c r="I113" s="27">
-        <f>H113-G113</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45802,7 +45802,7 @@
         <v>80</v>
       </c>
       <c r="D114" s="25">
-        <f>IF(NOT(ISBLANK(C114)), IF(ISNUMBER(C114), ROUND((C114 - 5)/20, 0), C114), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E114" s="26" t="s">
@@ -45821,7 +45821,7 @@
         <v>0</v>
       </c>
       <c r="I114" s="27">
-        <f>H114-G114</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45836,7 +45836,7 @@
         <v>80</v>
       </c>
       <c r="D115" s="25">
-        <f>IF(NOT(ISBLANK(C115)), IF(ISNUMBER(C115), ROUND((C115 - 5)/20, 0), C115), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E115" s="26" t="s">
@@ -45855,7 +45855,7 @@
         <v>0</v>
       </c>
       <c r="I115" s="27">
-        <f>H115-G115</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45870,7 +45870,7 @@
         <v>80</v>
       </c>
       <c r="D116" s="25">
-        <f>IF(NOT(ISBLANK(C116)), IF(ISNUMBER(C116), ROUND((C116 - 5)/20, 0), C116), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E116" s="26" t="s">
@@ -45889,7 +45889,7 @@
         <v>0</v>
       </c>
       <c r="I116" s="27">
-        <f>H116-G116</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45904,7 +45904,7 @@
         <v>80</v>
       </c>
       <c r="D117" s="25">
-        <f>IF(NOT(ISBLANK(C117)), IF(ISNUMBER(C117), ROUND((C117 - 5)/20, 0), C117), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E117" s="26" t="s">
@@ -45923,7 +45923,7 @@
         <v>0</v>
       </c>
       <c r="I117" s="27">
-        <f>H117-G117</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45938,7 +45938,7 @@
         <v>80</v>
       </c>
       <c r="D118" s="25">
-        <f>IF(NOT(ISBLANK(C118)), IF(ISNUMBER(C118), ROUND((C118 - 5)/20, 0), C118), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E118" s="26" t="s">
@@ -45957,7 +45957,7 @@
         <v>0</v>
       </c>
       <c r="I118" s="27">
-        <f>H118-G118</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -45972,7 +45972,7 @@
         <v>80</v>
       </c>
       <c r="D119" s="29">
-        <f>IF(NOT(ISBLANK(C119)), IF(ISNUMBER(C119), ROUND((C119 - 5)/20, 0), C119), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E119" s="26" t="s">
@@ -45991,7 +45991,7 @@
         <v>15</v>
       </c>
       <c r="I119" s="26">
-        <f>H119-G119</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46006,7 +46006,7 @@
         <v>90</v>
       </c>
       <c r="D120" s="29">
-        <f>IF(NOT(ISBLANK(C120)), IF(ISNUMBER(C120), ROUND((C120 - 5)/20, 0), C120), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E120" s="26" t="s">
@@ -46025,7 +46025,7 @@
         <v>17</v>
       </c>
       <c r="I120" s="26">
-        <f>H120-G120</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
@@ -46040,7 +46040,7 @@
         <v>80</v>
       </c>
       <c r="D121" s="29">
-        <f>IF(NOT(ISBLANK(C121)), IF(ISNUMBER(C121), ROUND((C121 - 5)/20, 0), C121), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E121" s="26" t="s">
@@ -46059,7 +46059,7 @@
         <v>20</v>
       </c>
       <c r="I121" s="26">
-        <f>H121-G121</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46074,7 +46074,7 @@
         <v>80</v>
       </c>
       <c r="D122" s="29">
-        <f>IF(NOT(ISBLANK(C122)), IF(ISNUMBER(C122), ROUND((C122 - 5)/20, 0), C122), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E122" s="26" t="s">
@@ -46093,7 +46093,7 @@
         <v>17</v>
       </c>
       <c r="I122" s="26">
-        <f>H122-G122</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46108,7 +46108,7 @@
         <v>80</v>
       </c>
       <c r="D123" s="29">
-        <f>IF(NOT(ISBLANK(C123)), IF(ISNUMBER(C123), ROUND((C123 - 5)/20, 0), C123), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E123" s="26" t="s">
@@ -46127,7 +46127,7 @@
         <v>16</v>
       </c>
       <c r="I123" s="26">
-        <f>H123-G123</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46142,7 +46142,7 @@
         <v>80</v>
       </c>
       <c r="D124" s="29">
-        <f>IF(NOT(ISBLANK(C124)), IF(ISNUMBER(C124), ROUND((C124 - 5)/20, 0), C124), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E124" s="26" t="s">
@@ -46161,7 +46161,7 @@
         <v>18</v>
       </c>
       <c r="I124" s="26">
-        <f>H124-G124</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -46176,7 +46176,7 @@
         <v>80</v>
       </c>
       <c r="D125" s="29">
-        <f>IF(NOT(ISBLANK(C125)), IF(ISNUMBER(C125), ROUND((C125 - 5)/20, 0), C125), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E125" s="26" t="s">
@@ -46195,7 +46195,7 @@
         <v>16</v>
       </c>
       <c r="I125" s="26">
-        <f>H125-G125</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46210,7 +46210,7 @@
         <v>75</v>
       </c>
       <c r="D126" s="29">
-        <f>IF(NOT(ISBLANK(C126)), IF(ISNUMBER(C126), ROUND((C126 - 5)/20, 0), C126), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E126" s="26" t="s">
@@ -46229,7 +46229,7 @@
         <v>18</v>
       </c>
       <c r="I126" s="26">
-        <f>H126-G126</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46244,7 +46244,7 @@
         <v>85</v>
       </c>
       <c r="D127" s="29">
-        <f>IF(NOT(ISBLANK(C127)), IF(ISNUMBER(C127), ROUND((C127 - 5)/20, 0), C127), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E127" s="26" t="s">
@@ -46263,7 +46263,7 @@
         <v>19</v>
       </c>
       <c r="I127" s="26">
-        <f>H127-G127</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -46278,7 +46278,7 @@
         <v>80</v>
       </c>
       <c r="D128" s="29">
-        <f>IF(NOT(ISBLANK(C128)), IF(ISNUMBER(C128), ROUND((C128 - 5)/20, 0), C128), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E128" s="26" t="s">
@@ -46297,7 +46297,7 @@
         <v>17</v>
       </c>
       <c r="I128" s="26">
-        <f>H128-G128</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46312,7 +46312,7 @@
         <v>80</v>
       </c>
       <c r="D129" s="29">
-        <f>IF(NOT(ISBLANK(C129)), IF(ISNUMBER(C129), ROUND((C129 - 5)/20, 0), C129), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E129" s="26" t="s">
@@ -46331,7 +46331,7 @@
         <v>17</v>
       </c>
       <c r="I129" s="26">
-        <f>H129-G129</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -46346,7 +46346,7 @@
         <v>80</v>
       </c>
       <c r="D130" s="29">
-        <f>IF(NOT(ISBLANK(C130)), IF(ISNUMBER(C130), ROUND((C130 - 5)/20, 0), C130), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E130" s="26" t="s">
@@ -46365,7 +46365,7 @@
         <v>19</v>
       </c>
       <c r="I130" s="26">
-        <f>H130-G130</f>
+        <f t="shared" ref="I130:I193" si="4">H130-G130</f>
         <v>3</v>
       </c>
     </row>
@@ -46380,7 +46380,7 @@
         <v>80</v>
       </c>
       <c r="D131" s="29">
-        <f>IF(NOT(ISBLANK(C131)), IF(ISNUMBER(C131), ROUND((C131 - 5)/20, 0), C131), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E131" s="26" t="s">
@@ -46399,7 +46399,7 @@
         <v>28</v>
       </c>
       <c r="I131" s="26">
-        <f>H131-G131</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46414,7 +46414,7 @@
         <v>90</v>
       </c>
       <c r="D132" s="29">
-        <f>IF(NOT(ISBLANK(C132)), IF(ISNUMBER(C132), ROUND((C132 - 5)/20, 0), C132), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E132" s="26" t="s">
@@ -46433,7 +46433,7 @@
         <v>19</v>
       </c>
       <c r="I132" s="26">
-        <f>H132-G132</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46448,7 +46448,7 @@
         <v>85</v>
       </c>
       <c r="D133" s="29">
-        <f>IF(NOT(ISBLANK(C133)), IF(ISNUMBER(C133), ROUND((C133 - 5)/20, 0), C133), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E133" s="26" t="s">
@@ -46467,7 +46467,7 @@
         <v>19</v>
       </c>
       <c r="I133" s="26">
-        <f>H133-G133</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -46482,7 +46482,7 @@
         <v>80</v>
       </c>
       <c r="D134" s="25">
-        <f>IF(NOT(ISBLANK(C134)), IF(ISNUMBER(C134), ROUND((C134 - 5)/20, 0), C134), "")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="E134" s="26" t="s">
@@ -46500,7 +46500,7 @@
         <v>19</v>
       </c>
       <c r="I134" s="27">
-        <f>H134-G134</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46515,7 +46515,7 @@
         <v>75</v>
       </c>
       <c r="D135" s="29">
-        <f>IF(NOT(ISBLANK(C135)), IF(ISNUMBER(C135), ROUND((C135 - 5)/20, 0), C135), "")</f>
+        <f t="shared" ref="D135:D198" si="5">IF(NOT(ISBLANK(C135)), IF(ISNUMBER(C135), ROUND((C135 - 5)/20, 0), C135), "")</f>
         <v>4</v>
       </c>
       <c r="E135" s="26" t="s">
@@ -46534,7 +46534,7 @@
         <v>18</v>
       </c>
       <c r="I135" s="26">
-        <f>H135-G135</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46549,7 +46549,7 @@
         <v>90</v>
       </c>
       <c r="D136" s="29">
-        <f>IF(NOT(ISBLANK(C136)), IF(ISNUMBER(C136), ROUND((C136 - 5)/20, 0), C136), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E136" s="26" t="s">
@@ -46568,7 +46568,7 @@
         <v>20</v>
       </c>
       <c r="I136" s="26">
-        <f>H136-G136</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46583,7 +46583,7 @@
         <v>80</v>
       </c>
       <c r="D137" s="29">
-        <f>IF(NOT(ISBLANK(C137)), IF(ISNUMBER(C137), ROUND((C137 - 5)/20, 0), C137), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E137" s="26" t="s">
@@ -46602,7 +46602,7 @@
         <v>18</v>
       </c>
       <c r="I137" s="26">
-        <f>H137-G137</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46617,7 +46617,7 @@
         <v>80</v>
       </c>
       <c r="D138" s="29">
-        <f>IF(NOT(ISBLANK(C138)), IF(ISNUMBER(C138), ROUND((C138 - 5)/20, 0), C138), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E138" s="26" t="s">
@@ -46636,7 +46636,7 @@
         <v>21</v>
       </c>
       <c r="I138" s="26">
-        <f>H138-G138</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -46651,7 +46651,7 @@
         <v>75</v>
       </c>
       <c r="D139" s="29">
-        <f>IF(NOT(ISBLANK(C139)), IF(ISNUMBER(C139), ROUND((C139 - 5)/20, 0), C139), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E139" s="26" t="s">
@@ -46670,7 +46670,7 @@
         <v>19</v>
       </c>
       <c r="I139" s="26">
-        <f>H139-G139</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
@@ -46685,7 +46685,7 @@
         <v>80</v>
       </c>
       <c r="D140" s="25">
-        <f>IF(NOT(ISBLANK(C140)), IF(ISNUMBER(C140), ROUND((C140 - 5)/20, 0), C140), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E140" s="26" t="s">
@@ -46704,7 +46704,7 @@
         <v>18</v>
       </c>
       <c r="I140" s="27">
-        <f>H140-G140</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46719,7 +46719,7 @@
         <v>80</v>
       </c>
       <c r="D141" s="29">
-        <f>IF(NOT(ISBLANK(C141)), IF(ISNUMBER(C141), ROUND((C141 - 5)/20, 0), C141), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E141" s="26" t="s">
@@ -46738,7 +46738,7 @@
         <v>28</v>
       </c>
       <c r="I141" s="26">
-        <f>H141-G141</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46753,7 +46753,7 @@
         <v>80</v>
       </c>
       <c r="D142" s="29">
-        <f>IF(NOT(ISBLANK(C142)), IF(ISNUMBER(C142), ROUND((C142 - 5)/20, 0), C142), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E142" s="26" t="s">
@@ -46772,7 +46772,7 @@
         <v>18</v>
       </c>
       <c r="I142" s="26">
-        <f>H142-G142</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -46787,7 +46787,7 @@
         <v>80</v>
       </c>
       <c r="D143" s="29">
-        <f>IF(NOT(ISBLANK(C143)), IF(ISNUMBER(C143), ROUND((C143 - 5)/20, 0), C143), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E143" s="26" t="s">
@@ -46806,7 +46806,7 @@
         <v>18</v>
       </c>
       <c r="I143" s="26">
-        <f>H143-G143</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -46821,7 +46821,7 @@
         <v>80</v>
       </c>
       <c r="D144" s="29">
-        <f>IF(NOT(ISBLANK(C144)), IF(ISNUMBER(C144), ROUND((C144 - 5)/20, 0), C144), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E144" s="26" t="s">
@@ -46840,7 +46840,7 @@
         <v>14</v>
       </c>
       <c r="I144" s="26">
-        <f>H144-G144</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46855,7 +46855,7 @@
         <v>90</v>
       </c>
       <c r="D145" s="29">
-        <f>IF(NOT(ISBLANK(C145)), IF(ISNUMBER(C145), ROUND((C145 - 5)/20, 0), C145), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E145" s="26" t="s">
@@ -46874,7 +46874,7 @@
         <v>17</v>
       </c>
       <c r="I145" s="26">
-        <f>H145-G145</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -46889,7 +46889,7 @@
         <v>75</v>
       </c>
       <c r="D146" s="29">
-        <f>IF(NOT(ISBLANK(C146)), IF(ISNUMBER(C146), ROUND((C146 - 5)/20, 0), C146), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E146" s="26" t="s">
@@ -46908,7 +46908,7 @@
         <v>14</v>
       </c>
       <c r="I146" s="26">
-        <f>H146-G146</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46923,7 +46923,7 @@
         <v>80</v>
       </c>
       <c r="D147" s="29">
-        <f>IF(NOT(ISBLANK(C147)), IF(ISNUMBER(C147), ROUND((C147 - 5)/20, 0), C147), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E147" s="26" t="s">
@@ -46942,7 +46942,7 @@
         <v>16</v>
       </c>
       <c r="I147" s="26">
-        <f>H147-G147</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -46957,7 +46957,7 @@
         <v>85</v>
       </c>
       <c r="D148" s="29">
-        <f>IF(NOT(ISBLANK(C148)), IF(ISNUMBER(C148), ROUND((C148 - 5)/20, 0), C148), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E148" s="26" t="s">
@@ -46976,7 +46976,7 @@
         <v>18</v>
       </c>
       <c r="I148" s="26">
-        <f>H148-G148</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -46991,7 +46991,7 @@
         <v>80</v>
       </c>
       <c r="D149" s="29">
-        <f>IF(NOT(ISBLANK(C149)), IF(ISNUMBER(C149), ROUND((C149 - 5)/20, 0), C149), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E149" s="26" t="s">
@@ -47010,7 +47010,7 @@
         <v>19</v>
       </c>
       <c r="I149" s="26">
-        <f>H149-G149</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47025,7 +47025,7 @@
         <v>75</v>
       </c>
       <c r="D150" s="29">
-        <f>IF(NOT(ISBLANK(C150)), IF(ISNUMBER(C150), ROUND((C150 - 5)/20, 0), C150), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E150" s="26" t="s">
@@ -47044,7 +47044,7 @@
         <v>14</v>
       </c>
       <c r="I150" s="26">
-        <f>H150-G150</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47059,7 +47059,7 @@
         <v>80</v>
       </c>
       <c r="D151" s="29">
-        <f>IF(NOT(ISBLANK(C151)), IF(ISNUMBER(C151), ROUND((C151 - 5)/20, 0), C151), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E151" s="26" t="s">
@@ -47078,7 +47078,7 @@
         <v>19</v>
       </c>
       <c r="I151" s="26">
-        <f>H151-G151</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47093,7 +47093,7 @@
         <v>85</v>
       </c>
       <c r="D152" s="29">
-        <f>IF(NOT(ISBLANK(C152)), IF(ISNUMBER(C152), ROUND((C152 - 5)/20, 0), C152), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E152" s="26" t="s">
@@ -47112,7 +47112,7 @@
         <v>17</v>
       </c>
       <c r="I152" s="26">
-        <f>H152-G152</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47127,7 +47127,7 @@
         <v>90</v>
       </c>
       <c r="D153" s="25">
-        <f>IF(NOT(ISBLANK(C153)), IF(ISNUMBER(C153), ROUND((C153 - 5)/20, 0), C153), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E153" s="26" t="s">
@@ -47146,7 +47146,7 @@
         <v>14</v>
       </c>
       <c r="I153" s="27">
-        <f>H153-G153</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47161,7 +47161,7 @@
         <v>75</v>
       </c>
       <c r="D154" s="25">
-        <f>IF(NOT(ISBLANK(C154)), IF(ISNUMBER(C154), ROUND((C154 - 5)/20, 0), C154), "")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="E154" s="26" t="s">
@@ -47180,7 +47180,7 @@
         <v>16</v>
       </c>
       <c r="I154" s="27">
-        <f>H154-G154</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47195,7 +47195,7 @@
         <v>100</v>
       </c>
       <c r="D155" s="29">
-        <f>IF(NOT(ISBLANK(C155)), IF(ISNUMBER(C155), ROUND((C155 - 5)/20, 0), C155), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E155" s="26" t="s">
@@ -47214,7 +47214,7 @@
         <v>0</v>
       </c>
       <c r="I155" s="26">
-        <f>H155-G155</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47229,7 +47229,7 @@
         <v>100</v>
       </c>
       <c r="D156" s="29">
-        <f>IF(NOT(ISBLANK(C156)), IF(ISNUMBER(C156), ROUND((C156 - 5)/20, 0), C156), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E156" s="26" t="s">
@@ -47248,7 +47248,7 @@
         <v>19</v>
       </c>
       <c r="I156" s="26">
-        <f>H156-G156</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47263,7 +47263,7 @@
         <v>100</v>
       </c>
       <c r="D157" s="29">
-        <f>IF(NOT(ISBLANK(C157)), IF(ISNUMBER(C157), ROUND((C157 - 5)/20, 0), C157), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E157" s="26" t="s">
@@ -47282,7 +47282,7 @@
         <v>19</v>
       </c>
       <c r="I157" s="26">
-        <f>H157-G157</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -47297,7 +47297,7 @@
         <v>100</v>
       </c>
       <c r="D158" s="29">
-        <f>IF(NOT(ISBLANK(C158)), IF(ISNUMBER(C158), ROUND((C158 - 5)/20, 0), C158), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E158" s="26" t="s">
@@ -47316,7 +47316,7 @@
         <v>17</v>
       </c>
       <c r="I158" s="26">
-        <f>H158-G158</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47331,7 +47331,7 @@
         <v>100</v>
       </c>
       <c r="D159" s="29">
-        <f>IF(NOT(ISBLANK(C159)), IF(ISNUMBER(C159), ROUND((C159 - 5)/20, 0), C159), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E159" s="26" t="s">
@@ -47350,7 +47350,7 @@
         <v>16</v>
       </c>
       <c r="I159" s="26">
-        <f>H159-G159</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47365,7 +47365,7 @@
         <v>100</v>
       </c>
       <c r="D160" s="29">
-        <f>IF(NOT(ISBLANK(C160)), IF(ISNUMBER(C160), ROUND((C160 - 5)/20, 0), C160), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E160" s="26" t="s">
@@ -47384,7 +47384,7 @@
         <v>18</v>
       </c>
       <c r="I160" s="26">
-        <f>H160-G160</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -47399,7 +47399,7 @@
         <v>100</v>
       </c>
       <c r="D161" s="29">
-        <f>IF(NOT(ISBLANK(C161)), IF(ISNUMBER(C161), ROUND((C161 - 5)/20, 0), C161), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E161" s="26" t="s">
@@ -47418,7 +47418,7 @@
         <v>21</v>
       </c>
       <c r="I161" s="26">
-        <f>H161-G161</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
@@ -47433,7 +47433,7 @@
         <v>95</v>
       </c>
       <c r="D162" s="29">
-        <f>IF(NOT(ISBLANK(C162)), IF(ISNUMBER(C162), ROUND((C162 - 5)/20, 0), C162), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E162" s="26" t="s">
@@ -47452,7 +47452,7 @@
         <v>23</v>
       </c>
       <c r="I162" s="26">
-        <f>H162-G162</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47467,7 +47467,7 @@
         <v>100</v>
       </c>
       <c r="D163" s="29">
-        <f>IF(NOT(ISBLANK(C163)), IF(ISNUMBER(C163), ROUND((C163 - 5)/20, 0), C163), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E163" s="26" t="s">
@@ -47486,7 +47486,7 @@
         <v>17</v>
       </c>
       <c r="I163" s="26">
-        <f>H163-G163</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -47501,7 +47501,7 @@
         <v>100</v>
       </c>
       <c r="D164" s="29">
-        <f>IF(NOT(ISBLANK(C164)), IF(ISNUMBER(C164), ROUND((C164 - 5)/20, 0), C164), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E164" s="26" t="s">
@@ -47520,7 +47520,7 @@
         <v>18</v>
       </c>
       <c r="I164" s="26">
-        <f>H164-G164</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47535,7 +47535,7 @@
         <v>100</v>
       </c>
       <c r="D165" s="29">
-        <f>IF(NOT(ISBLANK(C165)), IF(ISNUMBER(C165), ROUND((C165 - 5)/20, 0), C165), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E165" s="26" t="s">
@@ -47554,7 +47554,7 @@
         <v>18</v>
       </c>
       <c r="I165" s="26">
-        <f>H165-G165</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47569,7 +47569,7 @@
         <v>110</v>
       </c>
       <c r="D166" s="29">
-        <f>IF(NOT(ISBLANK(C166)), IF(ISNUMBER(C166), ROUND((C166 - 5)/20, 0), C166), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E166" s="26" t="s">
@@ -47588,7 +47588,7 @@
         <v>20</v>
       </c>
       <c r="I166" s="26">
-        <f>H166-G166</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -47603,7 +47603,7 @@
         <v>100</v>
       </c>
       <c r="D167" s="29">
-        <f>IF(NOT(ISBLANK(C167)), IF(ISNUMBER(C167), ROUND((C167 - 5)/20, 0), C167), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E167" s="26" t="s">
@@ -47622,7 +47622,7 @@
         <v>19</v>
       </c>
       <c r="I167" s="26">
-        <f>H167-G167</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47637,7 +47637,7 @@
         <v>100</v>
       </c>
       <c r="D168" s="29">
-        <f>IF(NOT(ISBLANK(C168)), IF(ISNUMBER(C168), ROUND((C168 - 5)/20, 0), C168), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E168" s="26" t="s">
@@ -47656,7 +47656,7 @@
         <v>19</v>
       </c>
       <c r="I168" s="26">
-        <f>H168-G168</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47671,7 +47671,7 @@
         <v>100</v>
       </c>
       <c r="D169" s="29">
-        <f>IF(NOT(ISBLANK(C169)), IF(ISNUMBER(C169), ROUND((C169 - 5)/20, 0), C169), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E169" s="26" t="s">
@@ -47690,7 +47690,7 @@
         <v>19</v>
       </c>
       <c r="I169" s="26">
-        <f>H169-G169</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47705,7 +47705,7 @@
         <v>100</v>
       </c>
       <c r="D170" s="29">
-        <f>IF(NOT(ISBLANK(C170)), IF(ISNUMBER(C170), ROUND((C170 - 5)/20, 0), C170), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E170" s="26" t="s">
@@ -47724,7 +47724,7 @@
         <v>19</v>
       </c>
       <c r="I170" s="26">
-        <f>H170-G170</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -47739,7 +47739,7 @@
         <v>100</v>
       </c>
       <c r="D171" s="29">
-        <f>IF(NOT(ISBLANK(C171)), IF(ISNUMBER(C171), ROUND((C171 - 5)/20, 0), C171), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E171" s="26" t="s">
@@ -47758,7 +47758,7 @@
         <v>20</v>
       </c>
       <c r="I171" s="26">
-        <f>H171-G171</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -47773,7 +47773,7 @@
         <v>100</v>
       </c>
       <c r="D172" s="29">
-        <f>IF(NOT(ISBLANK(C172)), IF(ISNUMBER(C172), ROUND((C172 - 5)/20, 0), C172), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E172" s="26" t="s">
@@ -47792,7 +47792,7 @@
         <v>19</v>
       </c>
       <c r="I172" s="26">
-        <f>H172-G172</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -47807,7 +47807,7 @@
         <v>100</v>
       </c>
       <c r="D173" s="29">
-        <f>IF(NOT(ISBLANK(C173)), IF(ISNUMBER(C173), ROUND((C173 - 5)/20, 0), C173), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E173" s="26" t="s">
@@ -47826,7 +47826,7 @@
         <v>20</v>
       </c>
       <c r="I173" s="26">
-        <f>H173-G173</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -47841,7 +47841,7 @@
         <v>100</v>
       </c>
       <c r="D174" s="29">
-        <f>IF(NOT(ISBLANK(C174)), IF(ISNUMBER(C174), ROUND((C174 - 5)/20, 0), C174), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E174" s="26" t="s">
@@ -47860,7 +47860,7 @@
         <v>20</v>
       </c>
       <c r="I174" s="26">
-        <f>H174-G174</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -47875,7 +47875,7 @@
         <v>95</v>
       </c>
       <c r="D175" s="29">
-        <f>IF(NOT(ISBLANK(C175)), IF(ISNUMBER(C175), ROUND((C175 - 5)/20, 0), C175), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E175" s="26" t="s">
@@ -47894,7 +47894,7 @@
         <v>18</v>
       </c>
       <c r="I175" s="26">
-        <f>H175-G175</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47909,7 +47909,7 @@
         <v>100</v>
       </c>
       <c r="D176" s="29">
-        <f>IF(NOT(ISBLANK(C176)), IF(ISNUMBER(C176), ROUND((C176 - 5)/20, 0), C176), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E176" s="26" t="s">
@@ -47928,7 +47928,7 @@
         <v>21</v>
       </c>
       <c r="I176" s="26">
-        <f>H176-G176</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -47943,7 +47943,7 @@
         <v>95</v>
       </c>
       <c r="D177" s="29">
-        <f>IF(NOT(ISBLANK(C177)), IF(ISNUMBER(C177), ROUND((C177 - 5)/20, 0), C177), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E177" s="26" t="s">
@@ -47962,7 +47962,7 @@
         <v>21</v>
       </c>
       <c r="I177" s="26">
-        <f>H177-G177</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -47977,7 +47977,7 @@
         <v>95</v>
       </c>
       <c r="D178" s="29">
-        <f>IF(NOT(ISBLANK(C178)), IF(ISNUMBER(C178), ROUND((C178 - 5)/20, 0), C178), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E178" s="26" t="s">
@@ -47996,7 +47996,7 @@
         <v>18</v>
       </c>
       <c r="I178" s="26">
-        <f>H178-G178</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48011,7 +48011,7 @@
         <v>95</v>
       </c>
       <c r="D179" s="29">
-        <f>IF(NOT(ISBLANK(C179)), IF(ISNUMBER(C179), ROUND((C179 - 5)/20, 0), C179), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E179" s="26" t="s">
@@ -48030,7 +48030,7 @@
         <v>17</v>
       </c>
       <c r="I179" s="26">
-        <f>H179-G179</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48045,7 +48045,7 @@
         <v>120</v>
       </c>
       <c r="D180" s="29">
-        <f>IF(NOT(ISBLANK(C180)), IF(ISNUMBER(C180), ROUND((C180 - 5)/20, 0), C180), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E180" s="26" t="s">
@@ -48064,7 +48064,7 @@
         <v>0</v>
       </c>
       <c r="I180" s="26">
-        <f>H180-G180</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48079,7 +48079,7 @@
         <v>110</v>
       </c>
       <c r="D181" s="29">
-        <f>IF(NOT(ISBLANK(C181)), IF(ISNUMBER(C181), ROUND((C181 - 5)/20, 0), C181), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E181" s="26" t="s">
@@ -48098,7 +48098,7 @@
         <v>19</v>
       </c>
       <c r="I181" s="26">
-        <f>H181-G181</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48113,7 +48113,7 @@
         <v>110</v>
       </c>
       <c r="D182" s="29">
-        <f>IF(NOT(ISBLANK(C182)), IF(ISNUMBER(C182), ROUND((C182 - 5)/20, 0), C182), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E182" s="26" t="s">
@@ -48132,7 +48132,7 @@
         <v>18</v>
       </c>
       <c r="I182" s="26">
-        <f>H182-G182</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48147,7 +48147,7 @@
         <v>110</v>
       </c>
       <c r="D183" s="29">
-        <f>IF(NOT(ISBLANK(C183)), IF(ISNUMBER(C183), ROUND((C183 - 5)/20, 0), C183), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E183" s="26" t="s">
@@ -48166,7 +48166,7 @@
         <v>17</v>
       </c>
       <c r="I183" s="27">
-        <f>H183-G183</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48181,7 +48181,7 @@
         <v>100</v>
       </c>
       <c r="D184" s="29">
-        <f>IF(NOT(ISBLANK(C184)), IF(ISNUMBER(C184), ROUND((C184 - 5)/20, 0), C184), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E184" s="26" t="s">
@@ -48200,7 +48200,7 @@
         <v>13</v>
       </c>
       <c r="I184" s="26">
-        <f>H184-G184</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -48215,7 +48215,7 @@
         <v>100</v>
       </c>
       <c r="D185" s="29">
-        <f>IF(NOT(ISBLANK(C185)), IF(ISNUMBER(C185), ROUND((C185 - 5)/20, 0), C185), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E185" s="26" t="s">
@@ -48234,7 +48234,7 @@
         <v>20</v>
       </c>
       <c r="I185" s="26">
-        <f>H185-G185</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48249,7 +48249,7 @@
         <v>100</v>
       </c>
       <c r="D186" s="29">
-        <f>IF(NOT(ISBLANK(C186)), IF(ISNUMBER(C186), ROUND((C186 - 5)/20, 0), C186), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E186" s="26" t="s">
@@ -48268,7 +48268,7 @@
         <v>23</v>
       </c>
       <c r="I186" s="26">
-        <f>H186-G186</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48283,7 +48283,7 @@
         <v>100</v>
       </c>
       <c r="D187" s="29">
-        <f>IF(NOT(ISBLANK(C187)), IF(ISNUMBER(C187), ROUND((C187 - 5)/20, 0), C187), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E187" s="26" t="s">
@@ -48302,7 +48302,7 @@
         <v>28</v>
       </c>
       <c r="I187" s="26">
-        <f>H187-G187</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48317,7 +48317,7 @@
         <v>100</v>
       </c>
       <c r="D188" s="29">
-        <f>IF(NOT(ISBLANK(C188)), IF(ISNUMBER(C188), ROUND((C188 - 5)/20, 0), C188), "")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="E188" s="26" t="s">
@@ -48336,7 +48336,7 @@
         <v>20</v>
       </c>
       <c r="I188" s="26">
-        <f>H188-G188</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48351,7 +48351,7 @@
         <v>115</v>
       </c>
       <c r="D189" s="25">
-        <f>IF(NOT(ISBLANK(C189)), IF(ISNUMBER(C189), ROUND((C189 - 5)/20, 0), C189), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E189" s="27" t="s">
@@ -48370,7 +48370,7 @@
         <v>17</v>
       </c>
       <c r="I189" s="27">
-        <f>H189-G189</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48385,7 +48385,7 @@
         <v>120</v>
       </c>
       <c r="D190" s="29">
-        <f>IF(NOT(ISBLANK(C190)), IF(ISNUMBER(C190), ROUND((C190 - 5)/20, 0), C190), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E190" s="26" t="s">
@@ -48404,7 +48404,7 @@
         <v>18</v>
       </c>
       <c r="I190" s="26">
-        <f>H190-G190</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -48419,7 +48419,7 @@
         <v>120</v>
       </c>
       <c r="D191" s="29">
-        <f>IF(NOT(ISBLANK(C191)), IF(ISNUMBER(C191), ROUND((C191 - 5)/20, 0), C191), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E191" s="26" t="s">
@@ -48438,7 +48438,7 @@
         <v>18</v>
       </c>
       <c r="I191" s="26">
-        <f>H191-G191</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48453,7 +48453,7 @@
         <v>120</v>
       </c>
       <c r="D192" s="29">
-        <f>IF(NOT(ISBLANK(C192)), IF(ISNUMBER(C192), ROUND((C192 - 5)/20, 0), C192), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E192" s="26" t="s">
@@ -48472,7 +48472,7 @@
         <v>28</v>
       </c>
       <c r="I192" s="26">
-        <f>H192-G192</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48487,7 +48487,7 @@
         <v>120</v>
       </c>
       <c r="D193" s="25">
-        <f>IF(NOT(ISBLANK(C193)), IF(ISNUMBER(C193), ROUND((C193 - 5)/20, 0), C193), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E193" s="26" t="s">
@@ -48506,7 +48506,7 @@
         <v>0</v>
       </c>
       <c r="I193" s="27">
-        <f>H193-G193</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -48521,7 +48521,7 @@
         <v>120</v>
       </c>
       <c r="D194" s="25">
-        <f>IF(NOT(ISBLANK(C194)), IF(ISNUMBER(C194), ROUND((C194 - 5)/20, 0), C194), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E194" s="26" t="s">
@@ -48540,7 +48540,7 @@
         <v>0</v>
       </c>
       <c r="I194" s="27">
-        <f>H194-G194</f>
+        <f t="shared" ref="I194:I257" si="6">H194-G194</f>
         <v>0</v>
       </c>
     </row>
@@ -48555,7 +48555,7 @@
         <v>120</v>
       </c>
       <c r="D195" s="29">
-        <f>IF(NOT(ISBLANK(C195)), IF(ISNUMBER(C195), ROUND((C195 - 5)/20, 0), C195), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E195" s="26" t="s">
@@ -48574,7 +48574,7 @@
         <v>19</v>
       </c>
       <c r="I195" s="26">
-        <f>H195-G195</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48589,7 +48589,7 @@
         <v>120</v>
       </c>
       <c r="D196" s="25">
-        <f>IF(NOT(ISBLANK(C196)), IF(ISNUMBER(C196), ROUND((C196 - 5)/20, 0), C196), "")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="E196" s="27" t="s">
@@ -48608,7 +48608,7 @@
         <v>17</v>
       </c>
       <c r="I196" s="27">
-        <f>H196-G196</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48623,7 +48623,7 @@
         <v>150</v>
       </c>
       <c r="D197" s="25">
-        <f>IF(NOT(ISBLANK(C197)), IF(ISNUMBER(C197), ROUND((C197 - 5)/20, 0), C197), "")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="E197" s="27" t="s">
@@ -48642,7 +48642,7 @@
         <v>0</v>
       </c>
       <c r="I197" s="27">
-        <f>H197-G197</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48657,7 +48657,7 @@
         <v>150</v>
       </c>
       <c r="D198" s="29">
-        <f>IF(NOT(ISBLANK(C198)), IF(ISNUMBER(C198), ROUND((C198 - 5)/20, 0), C198), "")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="E198" s="26" t="s">
@@ -48676,7 +48676,7 @@
         <v>23</v>
       </c>
       <c r="I198" s="26">
-        <f>H198-G198</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48691,7 +48691,7 @@
         <v>519</v>
       </c>
       <c r="D199" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C199)), IF(ISNUMBER(C199), ROUND((C199 - 5)/20, 0), C199), "")</f>
+        <f t="shared" ref="D199:D262" si="7">IF(NOT(ISBLANK(C199)), IF(ISNUMBER(C199), ROUND((C199 - 5)/20, 0), C199), "")</f>
         <v>?</v>
       </c>
       <c r="E199" s="26" t="s">
@@ -48710,7 +48710,7 @@
         <v>20</v>
       </c>
       <c r="I199" s="26">
-        <f>H199-G199</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48725,7 +48725,7 @@
         <v>519</v>
       </c>
       <c r="D200" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C200)), IF(ISNUMBER(C200), ROUND((C200 - 5)/20, 0), C200), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E200" s="26" t="s">
@@ -48744,7 +48744,7 @@
         <v>18</v>
       </c>
       <c r="I200" s="26">
-        <f>H200-G200</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48759,7 +48759,7 @@
         <v>519</v>
       </c>
       <c r="D201" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C201)), IF(ISNUMBER(C201), ROUND((C201 - 5)/20, 0), C201), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E201" s="26" t="s">
@@ -48778,7 +48778,7 @@
         <v>20</v>
       </c>
       <c r="I201" s="26">
-        <f>H201-G201</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -48793,7 +48793,7 @@
         <v>519</v>
       </c>
       <c r="D202" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C202)), IF(ISNUMBER(C202), ROUND((C202 - 5)/20, 0), C202), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E202" s="26" t="s">
@@ -48812,7 +48812,7 @@
         <v>18</v>
       </c>
       <c r="I202" s="26">
-        <f>H202-G202</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48827,7 +48827,7 @@
         <v>519</v>
       </c>
       <c r="D203" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C203)), IF(ISNUMBER(C203), ROUND((C203 - 5)/20, 0), C203), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E203" s="26" t="s">
@@ -48846,7 +48846,7 @@
         <v>14</v>
       </c>
       <c r="I203" s="26">
-        <f>H203-G203</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48861,7 +48861,7 @@
         <v>519</v>
       </c>
       <c r="D204" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C204)), IF(ISNUMBER(C204), ROUND((C204 - 5)/20, 0), C204), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E204" s="26" t="s">
@@ -48880,7 +48880,7 @@
         <v>12</v>
       </c>
       <c r="I204" s="26">
-        <f>H204-G204</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48895,7 +48895,7 @@
         <v>519</v>
       </c>
       <c r="D205" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C205)), IF(ISNUMBER(C205), ROUND((C205 - 5)/20, 0), C205), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E205" s="26" t="s">
@@ -48914,7 +48914,7 @@
         <v>18</v>
       </c>
       <c r="I205" s="26">
-        <f>H205-G205</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48929,7 +48929,7 @@
         <v>519</v>
       </c>
       <c r="D206" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C206)), IF(ISNUMBER(C206), ROUND((C206 - 5)/20, 0), C206), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E206" s="26" t="s">
@@ -48948,7 +48948,7 @@
         <v>11</v>
       </c>
       <c r="I206" s="26">
-        <f>H206-G206</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48963,7 +48963,7 @@
         <v>519</v>
       </c>
       <c r="D207" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C207)), IF(ISNUMBER(C207), ROUND((C207 - 5)/20, 0), C207), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E207" s="26" t="s">
@@ -48982,7 +48982,7 @@
         <v>11</v>
       </c>
       <c r="I207" s="26">
-        <f>H207-G207</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -48997,7 +48997,7 @@
         <v>519</v>
       </c>
       <c r="D208" s="29" t="str">
-        <f>IF(NOT(ISBLANK(C208)), IF(ISNUMBER(C208), ROUND((C208 - 5)/20, 0), C208), "")</f>
+        <f t="shared" si="7"/>
         <v>?</v>
       </c>
       <c r="E208" s="26" t="s">
@@ -49016,7 +49016,7 @@
         <v>11</v>
       </c>
       <c r="I208" s="26">
-        <f>H208-G208</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>